<commit_message>
feat: update file output peringkat
</commit_message>
<xml_diff>
--- a/peringkat.xlsx
+++ b/peringkat.xlsx
@@ -418,27 +418,27 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C2">
-        <v>22825</v>
+        <v>34513</v>
       </c>
       <c r="D2">
-        <v>90</v>
+        <v>90.00000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3">
-        <v>24704</v>
+        <v>34107</v>
       </c>
       <c r="D3">
         <v>90</v>
@@ -446,13 +446,13 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4">
-        <v>20052</v>
+        <v>35119</v>
       </c>
       <c r="D4">
         <v>90</v>
@@ -460,13 +460,13 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C5">
-        <v>24551</v>
+        <v>39211</v>
       </c>
       <c r="D5">
         <v>90</v>
@@ -474,13 +474,13 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C6">
-        <v>27315</v>
+        <v>22825</v>
       </c>
       <c r="D6">
         <v>90</v>

</xml_diff>